<commit_message>
- updated case - added script
</commit_message>
<xml_diff>
--- a/cases/case_2_bi_report/data/supplier.xlsx
+++ b/cases/case_2_bi_report/data/supplier.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10604"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jan/Projects/01_courses/ppa-erp/create_dataset/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jan/Documents/02_teaching/fau/course_business_analytics_students/cases/case_2_bi_report/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B70944C-4284-B248-A91E-AEF2FC908D20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D330EAA6-5E7C-494F-B408-892DEFDC5C68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="36660" yWindow="8380" windowWidth="28040" windowHeight="17440" xr2:uid="{A5533BA7-ABB9-4249-A0F7-D2C0F80D3EC5}"/>
   </bookViews>
@@ -660,7 +660,7 @@
   <dimension ref="A1:I16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>